<commit_message>
Rework power system for hybrid cap and bq25770
</commit_message>
<xml_diff>
--- a/PCB/PCBv1.3/bq25505 calc.xlsx
+++ b/PCB/PCBv1.3/bq25505 calc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Veridian-Heliograph\PCB\PCBv1.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Veridian-Heliograph\PCB\PCBv1.3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E355ED0-818E-45BC-9886-6B9F6A72EB0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6E983A-DC40-435D-9A6B-FE6D93208385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2985" yWindow="2985" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21600" yWindow="18840" windowWidth="21810" windowHeight="18840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bq25505(70" sheetId="1" r:id="rId1"/>
@@ -2232,9 +2232,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C23" sqref="C23"/>
+      <selection pane="topRight" activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2456,7 +2456,7 @@
         <v>8</v>
       </c>
       <c r="I8" s="13">
-        <v>1.9</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>1</v>
@@ -2498,7 +2498,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="13">
-        <v>5.5</v>
+        <v>3.8</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>1</v>
@@ -2509,7 +2509,7 @@
         <v>20</v>
       </c>
       <c r="I9" s="13">
-        <v>2.2999999999999998</v>
+        <v>2.9</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>1</v>
@@ -2522,7 +2522,7 @@
         <v>44</v>
       </c>
       <c r="O9" s="13">
-        <v>1.8</v>
+        <v>3</v>
       </c>
       <c r="P9" s="4" t="s">
         <v>1</v>
@@ -2649,15 +2649,15 @@
       </c>
       <c r="I13" s="31">
         <f>C1/I9*I7</f>
-        <v>6.8391304347826098</v>
+        <v>5.4241379310344824</v>
       </c>
       <c r="J13" s="52">
         <f>IF(I13&gt;1,VLOOKUP(I13*10,$AA$27:$AA$133,1)/10,IF(I13&gt;0.099,VLOOKUP(I13*100,$AB$27:$AB$133,1)/100,VLOOKUP(I13*1000,$AB$27:$AB$133,1)/1000))</f>
-        <v>6.81</v>
+        <v>5.36</v>
       </c>
       <c r="K13" s="52">
         <f ca="1">IF(I13&gt;1,OFFSET($AA$27,MATCH(I13*10,$AA$27:$AA$133,1),0)/10,IF(I13&gt;0.099, OFFSET($AB$27,MATCH(I13*100,$AB$27:$AB$133,1),0)/100,OFFSET($AB$27,MATCH(I13*1000,$AB$27:$AB$133,1),0)/1000))</f>
-        <v>6.9799999999999995</v>
+        <v>5.49</v>
       </c>
       <c r="L13" s="54" t="s">
         <v>59</v>
@@ -2701,15 +2701,15 @@
       </c>
       <c r="C14" s="31">
         <f>C8*$C$1/C9*3/2</f>
-        <v>4.29</v>
+        <v>6.2092105263157897</v>
       </c>
       <c r="D14" s="52">
         <f>IF(C14&gt;1,VLOOKUP(C14*10,$AA$27:$AA$133,1)/10,IF(C14&gt;0.099,VLOOKUP(C14*100,$AB$27:$AB$133,1)/100,VLOOKUP(C14*1000,$AB$27:$AB$133,1)/1000))</f>
-        <v>4.2200000000000006</v>
+        <v>6.1899999999999995</v>
       </c>
       <c r="E14" s="52">
         <f ca="1">IF(C14&gt;1,OFFSET($AA$27,MATCH(C14*10,$AA$27:$AA$133,1),0)/10,IF(C14&gt;0.099, OFFSET($AB$27,MATCH(C14*100,$AB$27:$AB$133,1),0)/100,OFFSET($AB$27,MATCH(C14*1000,$AB$27:$AB$133,1),0)/1000))</f>
-        <v>4.32</v>
+        <v>6.34</v>
       </c>
       <c r="F14" s="54" t="s">
         <v>59</v>
@@ -2719,15 +2719,15 @@
       </c>
       <c r="I14" s="31">
         <f>(I8/C1-1)*I13</f>
-        <v>3.9</v>
+        <v>4.4379310344827596</v>
       </c>
       <c r="J14" s="52">
         <f>IF(I14&gt;1,VLOOKUP(I14*10,$AA$27:$AA$133,1)/10,IF(I14&gt;0.099,VLOOKUP(I14*100,$AB$27:$AB$133,1)/100,VLOOKUP(I14*1000,$AB$27:$AB$133,1)/1000))</f>
-        <v>3.8299999999999996</v>
+        <v>4.42</v>
       </c>
       <c r="K14" s="52">
         <f ca="1">IF(I14&gt;1,OFFSET($AA$27,MATCH(I14*10,$AA$27:$AA$133,1),0)/10,IF(I14&gt;0.099, OFFSET($AB$27,MATCH(I14*100,$AB$27:$AB$133,1),0)/100,OFFSET($AB$27,MATCH(I14*1000,$AB$27:$AB$133,1),0)/1000))</f>
-        <v>3.9200000000000004</v>
+        <v>4.5299999999999994</v>
       </c>
       <c r="L14" s="54" t="s">
         <v>59</v>
@@ -2737,15 +2737,15 @@
       </c>
       <c r="O14" s="31">
         <f>IF(O8*$C$1/O9&lt;=10, O8*$C$1/O9, O8*$C$1/O9-10)</f>
-        <v>8.7388888888888889</v>
+        <v>5.2433333333333332</v>
       </c>
       <c r="P14" s="52">
         <f>IF(O14&gt;1,VLOOKUP(O14*10,$AA$26:$AA$132,1)/10,IF(O14&gt;0.099,VLOOKUP(O14*100,$AB$26:$AB$132,1)/100,VLOOKUP(O14*1000,$AB$26:$AB$132,1)/1000))</f>
-        <v>8.66</v>
+        <v>5.2299999999999995</v>
       </c>
       <c r="Q14" s="52">
         <f ca="1">IF(O14&gt;1,OFFSET($AA$26,MATCH(O14*10,$AA$26:$AA$132,1),0)/10,IF(O14&gt;0.099, OFFSET($AB$26,MATCH(O14*100,$AB$26:$AB$132,1),0)/100,OFFSET($AB$26,MATCH(O14*1000,$AB$26:$AB$132,1),0)/1000))</f>
-        <v>8.870000000000001</v>
+        <v>5.36</v>
       </c>
       <c r="R14" s="54" t="s">
         <v>59</v>
@@ -2778,15 +2778,15 @@
       </c>
       <c r="C15" s="31">
         <f>C8-C14</f>
-        <v>8.7100000000000009</v>
+        <v>6.7907894736842103</v>
       </c>
       <c r="D15" s="52">
         <f>IF(C15&gt;1,VLOOKUP(C15*10,$AA$27:$AA$133,1)/10,IF(C15&gt;0.099,VLOOKUP(C15*100,$AB$27:$AB$133,1)/100,VLOOKUP(C15*1000,$AB$27:$AB$133,1)/1000))</f>
-        <v>8.66</v>
+        <v>6.65</v>
       </c>
       <c r="E15" s="52">
         <f ca="1">IF(C15&gt;1,OFFSET($AA$27,MATCH(C15*10,$AA$27:$AA$133,1),0)/10,IF(C15&gt;0.099, OFFSET($AB$27,MATCH(C15*100,$AB$27:$AB$133,1),0)/100,OFFSET($AB$27,MATCH(C15*1000,$AB$27:$AB$133,1),0)/1000))</f>
-        <v>8.870000000000001</v>
+        <v>6.81</v>
       </c>
       <c r="F15" s="54" t="s">
         <v>59</v>
@@ -2796,15 +2796,15 @@
       </c>
       <c r="I15" s="31">
         <f>I7-I13-I14</f>
-        <v>2.2608695652173902</v>
+        <v>3.137931034482758</v>
       </c>
       <c r="J15" s="52">
         <f>IF(I15&gt;1,VLOOKUP(I15*10,$AA$27:$AA$133,1)/10,IF(I15&gt;0.099,VLOOKUP(I15*100,$AB$27:$AB$133,1)/100,VLOOKUP(I15*1000,$AB$27:$AB$133,1)/1000))</f>
-        <v>2.2600000000000002</v>
+        <v>3.09</v>
       </c>
       <c r="K15" s="52">
         <f ca="1">IF(I15&gt;1,OFFSET($AA$27,MATCH(I15*10,$AA$27:$AA$133,1),0)/10,IF(I15&gt;0.099, OFFSET($AB$27,MATCH(I15*100,$AB$27:$AB$133,1),0)/100,OFFSET($AB$27,MATCH(I15*1000,$AB$27:$AB$133,1),0)/1000))</f>
-        <v>2.3199999999999998</v>
+        <v>3.16</v>
       </c>
       <c r="L15" s="54" t="s">
         <v>59</v>
@@ -2856,11 +2856,11 @@
       <c r="C16" s="32"/>
       <c r="D16" s="53">
         <f>C1*(1+D15/D14)*3/2</f>
-        <v>5.5396208530805673</v>
+        <v>3.7648788368336028</v>
       </c>
       <c r="E16" s="53">
         <f ca="1">C1*(1+E15/E14)*3/2</f>
-        <v>5.5416319444444451</v>
+        <v>3.7645504731861195</v>
       </c>
       <c r="F16" s="83" t="s">
         <v>1</v>
@@ -2871,11 +2871,11 @@
       <c r="I16" s="18"/>
       <c r="J16" s="53">
         <f>C1*(1+J14/J13)</f>
-        <v>1.8905139500734214</v>
+        <v>2.2077985074626865</v>
       </c>
       <c r="K16" s="53">
         <f ca="1">C1*(1+K14/K13)</f>
-        <v>1.8895415472779371</v>
+        <v>2.2084153005464477</v>
       </c>
       <c r="L16" s="83" t="s">
         <v>1</v>
@@ -2885,15 +2885,15 @@
       </c>
       <c r="O16" s="31">
         <f>IF(O8*$C$1/O9&lt;=10, O8-O14, O8-O14-10)</f>
-        <v>4.2611111111111111</v>
+        <v>7.7566666666666668</v>
       </c>
       <c r="P16" s="52">
         <f>IF(O16&gt;1,VLOOKUP(O16*10,$AA$26:$AA$132,1)/10,IF(O16&gt;0.099,VLOOKUP(O16*100,$AB$26:$AB$132,1)/100,VLOOKUP(O16*1000,$AB$26:$AB$132,1)/1000))</f>
-        <v>4.2200000000000006</v>
+        <v>7.68</v>
       </c>
       <c r="Q16" s="52">
         <f ca="1">IF(O16&gt;1,OFFSET($AA$26,MATCH(O16*10,$AA$26:$AA$132,1),0)/10,IF(O16&gt;0.099, OFFSET($AB$26,MATCH(O16*100,$AB$26:$AB$132,1),0)/100,OFFSET($AB$26,MATCH(O16*1000,$AB$26:$AB$132,1),0)/1000))</f>
-        <v>4.32</v>
+        <v>7.87</v>
       </c>
       <c r="R16" s="54" t="s">
         <v>59</v>
@@ -2932,11 +2932,11 @@
       <c r="I17" s="18"/>
       <c r="J17" s="53">
         <f>(C1*((J13+J14+J15)/J13))</f>
-        <v>2.2920704845814974</v>
+        <v>2.9053544776119402</v>
       </c>
       <c r="K17" s="60">
         <f ca="1">(C1*((K13+K14+K15)/K13))</f>
-        <v>2.2917191977077365</v>
+        <v>2.9048816029143896</v>
       </c>
       <c r="L17" s="83" t="s">
         <v>1</v>
@@ -2947,11 +2947,11 @@
       <c r="O17" s="18"/>
       <c r="P17" s="53">
         <f>$C$1*(1+P16/(P14+P15))</f>
-        <v>1.7996304849884528</v>
+        <v>2.9868260038240919</v>
       </c>
       <c r="Q17" s="53">
         <f ca="1">$C$1*(1+Q16/(Q14+Q15))</f>
-        <v>1.7993122886133033</v>
+        <v>2.986623134328358</v>
       </c>
       <c r="R17" s="92" t="s">
         <v>1</v>
@@ -3003,7 +3003,7 @@
         <v>15</v>
       </c>
       <c r="C19" s="13">
-        <v>4.3</v>
+        <v>6.34</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>58</v>
@@ -3014,7 +3014,7 @@
         <v>17</v>
       </c>
       <c r="I19" s="13">
-        <v>6.81</v>
+        <v>5.36</v>
       </c>
       <c r="J19" s="4" t="s">
         <v>58</v>
@@ -3025,7 +3025,7 @@
         <v>45</v>
       </c>
       <c r="O19" s="13">
-        <v>8.66</v>
+        <v>5.36</v>
       </c>
       <c r="P19" s="4" t="s">
         <v>58</v>
@@ -3052,7 +3052,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="13">
-        <v>8.66</v>
+        <v>6.34</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>58</v>
@@ -3063,7 +3063,7 @@
         <v>18</v>
       </c>
       <c r="I20" s="13">
-        <v>3.83</v>
+        <v>4.42</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>58</v>
@@ -3108,7 +3108,7 @@
         <v>19</v>
       </c>
       <c r="I21" s="13">
-        <v>2.2599999999999998</v>
+        <v>3.09</v>
       </c>
       <c r="J21" s="4" t="s">
         <v>58</v>
@@ -3119,7 +3119,7 @@
         <v>46</v>
       </c>
       <c r="O21" s="13">
-        <v>4.32</v>
+        <v>7.87</v>
       </c>
       <c r="P21" s="4" t="s">
         <v>58</v>
@@ -3177,14 +3177,14 @@
       </c>
       <c r="C23" s="64">
         <f>$C$1*(1+C20/C19)*3/2</f>
-        <v>5.4703255813953486</v>
+        <v>3.63</v>
       </c>
       <c r="D23" s="86" t="s">
         <v>1</v>
       </c>
       <c r="E23" s="65">
         <f>(C23-C9)/C23*100</f>
-        <v>-0.54246165357276832</v>
+        <v>-4.6831955922864994</v>
       </c>
       <c r="F23" s="84" t="s">
         <v>2</v>
@@ -3194,14 +3194,14 @@
       </c>
       <c r="I23" s="64">
         <f>C1*(1+I20/I19)</f>
-        <v>1.8905139500734216</v>
+        <v>2.2077985074626865</v>
       </c>
       <c r="J23" s="79" t="s">
         <v>1</v>
       </c>
       <c r="K23" s="65">
         <f>(I23-I8)/I23*100</f>
-        <v>-0.50177095631639757</v>
+        <v>0.35322550659972712</v>
       </c>
       <c r="L23" s="84" t="s">
         <v>2</v>
@@ -3211,11 +3211,11 @@
       </c>
       <c r="O23" s="64">
         <f>$C$1*(1+O21/(O19+O20))</f>
-        <v>1.8136027713625866</v>
+        <v>2.986623134328358</v>
       </c>
       <c r="P23" s="65">
         <f>(O23-O9)/O23*100</f>
-        <v>0.75004138598479431</v>
+        <v>-0.44789265568486986</v>
       </c>
       <c r="Q23" s="94" t="s">
         <v>2</v>
@@ -3241,14 +3241,14 @@
       </c>
       <c r="I24" s="77">
         <f>(C1*((I19+I20+I21)/I19))</f>
-        <v>2.2920704845814979</v>
+        <v>2.9053544776119402</v>
       </c>
       <c r="J24" s="97" t="s">
         <v>1</v>
       </c>
       <c r="K24" s="78">
         <f>(I24-I9)/I24*100</f>
-        <v>-0.34595425715932027</v>
+        <v>0.18429687851175464</v>
       </c>
       <c r="L24" s="82" t="s">
         <v>2</v>
@@ -4274,24 +4274,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Tag xmlns="e6b6f262-197a-43d7-8cc8-2398f9beca90" xsi:nil="true"/>
-    <Thumbnail xmlns="e6b6f262-197a-43d7-8cc8-2398f9beca90" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000F22CD293BA2654895D1449C225927AC" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d0bb95fcecff743878fa884d2d9e7463">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e6b6f262-197a-43d7-8cc8-2398f9beca90" xmlns:ns3="236af784-b296-4cea-a5d3-eed352c284c4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3ea284607afbf8a45488423d608757b4" ns2:_="" ns3:_="">
     <xsd:import namespace="e6b6f262-197a-43d7-8cc8-2398f9beca90"/>
@@ -4528,25 +4510,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{455C7BEF-6E75-4721-857D-8DB037DB4B67}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Tag xmlns="e6b6f262-197a-43d7-8cc8-2398f9beca90" xsi:nil="true"/>
+    <Thumbnail xmlns="e6b6f262-197a-43d7-8cc8-2398f9beca90" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{276C0D19-B21D-4E63-AC38-166F7A170215}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e6b6f262-197a-43d7-8cc8-2398f9beca90"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C222E574-9BC3-4968-98EC-66C15D13800B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4563,4 +4545,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{276C0D19-B21D-4E63-AC38-166F7A170215}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e6b6f262-197a-43d7-8cc8-2398f9beca90"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{455C7BEF-6E75-4721-857D-8DB037DB4B67}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>